<commit_message>
Data Import, AI for excel
</commit_message>
<xml_diff>
--- a/Excel/Other/Session7_Solution.xlsx
+++ b/Excel/Other/Session7_Solution.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\07_Videos\01_excel\Excercise\Excercise\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ds_30\Excel\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05A6D0DF-21E4-453F-A1C2-F571087DB550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6915" tabRatio="696"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercise" sheetId="3" r:id="rId1"/>
@@ -152,7 +153,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1198,22 +1199,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.5">
       <c r="B2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>24</v>
       </c>
@@ -1228,7 +1231,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1241,7 +1244,7 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
     </row>
-    <row r="6" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -1258,7 +1261,7 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
     </row>
-    <row r="7" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -1275,7 +1278,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
     </row>
-    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -1292,7 +1295,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
     </row>
-    <row r="9" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4">
         <v>4</v>
       </c>
@@ -1309,7 +1312,7 @@
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
     </row>
-    <row r="10" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B10" s="4">
         <v>5</v>
       </c>
@@ -1326,7 +1329,7 @@
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B11" s="4">
         <v>6</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B12" s="4">
         <v>7</v>
       </c>
@@ -1342,7 +1345,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B13" s="4">
         <v>8</v>
       </c>
@@ -1350,7 +1353,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B14" s="4">
         <v>9</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B15" s="4">
         <v>10</v>
       </c>
@@ -1366,7 +1369,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:12" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B16" s="4">
         <v>11</v>
       </c>
@@ -1441,26 +1444,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane xSplit="2" ySplit="4" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" ht="19" x14ac:dyDescent="0.4">
       <c r="B3" s="14" t="s">
         <v>26</v>
       </c>
@@ -1470,7 +1473,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
         <v>7</v>
       </c>
@@ -1490,7 +1493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1510,7 +1513,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1530,7 +1533,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B8" s="5" t="s">
         <v>12</v>
       </c>
@@ -1570,7 +1573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
@@ -1590,7 +1593,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1610,7 +1613,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1630,7 +1633,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1650,7 +1653,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1690,7 +1693,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B15" s="8" t="s">
         <v>18</v>
       </c>

</xml_diff>